<commit_message>
add new data to Sistema de Notificacion de Muertes Violentas
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Sistema_de_Notificacion_de_Muertes_Violentas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0983C0-333A-5941-A0F3-8940210ACF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C44735D0-6C80-4321-A630-D674F0DA39C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320" xr2:uid="{158DB65A-6E55-0941-A295-AA375E07226E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
     <t>Grupo de edad</t>
   </si>
   <si>
-    <t>Total</t>
+    <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t>Menos de 15 años</t>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,9 +121,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,9 +145,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -182,7 +185,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -288,7 +291,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA841438-AD1F-5942-BFE3-B2D151D6E29E}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,11 +468,14 @@
       <c r="F1" s="1">
         <v>2021</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -485,14 +491,18 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <f>SUM(B2:G2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -508,14 +518,18 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <f>SUM(B3:G3)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -531,14 +545,18 @@
       <c r="E4">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>7</v>
       </c>
-      <c r="G4" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H3:H14" si="0">SUM(B4:G4)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,14 +572,18 @@
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="F5" s="1">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="2">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -577,14 +599,18 @@
       <c r="E6">
         <v>6</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -600,14 +626,18 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -623,14 +653,18 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="1">
-        <v>4</v>
-      </c>
-      <c r="G8" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -646,14 +680,18 @@
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -669,14 +707,18 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -692,14 +734,18 @@
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -713,13 +759,20 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -735,29 +788,48 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="G13">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
+        <f>SUM(B2:B13)</f>
         <v>36</v>
       </c>
       <c r="C14">
+        <f>SUM(C2:C13)</f>
         <v>53</v>
       </c>
       <c r="D14">
+        <f>SUM(D2:D13)</f>
         <v>41</v>
       </c>
       <c r="E14">
-        <v>48</v>
-      </c>
-      <c r="G14">
+        <f>SUM(E2:E13)</f>
+        <v>49</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" ref="F14:H14" si="1">SUM(F2:F13)</f>
+        <v>37</v>
+      </c>
+      <c r="G14" s="2">
         <f>SUM(G2:G13)</f>
-        <v>211</v>
+        <v>53</v>
+      </c>
+      <c r="H14" s="2">
+        <f>SUM(H2:H13)</f>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data for 2023 in SNMV
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Sistema_de_Notificacion_de_Muertes_Violentas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C44735D0-6C80-4321-A630-D674F0DA39C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7471904-2355-45F9-8456-7E7BBCF1E4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320" xr2:uid="{158DB65A-6E55-0941-A295-AA375E07226E}"/>
   </bookViews>
@@ -441,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA841438-AD1F-5942-BFE3-B2D151D6E29E}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,11 +471,14 @@
       <c r="G1" s="2">
         <v>2022</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="H1" s="2">
+        <v>2023</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -498,11 +501,14 @@
         <v>1</v>
       </c>
       <c r="H2" s="2">
-        <f>SUM(B2:G2)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <f>SUM(B2:H2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -525,11 +531,14 @@
         <v>4</v>
       </c>
       <c r="H3" s="2">
-        <f>SUM(B3:G3)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -552,11 +561,14 @@
         <v>4</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H3:H14" si="0">SUM(B4:G4)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -579,11 +591,14 @@
         <v>10</v>
       </c>
       <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -606,11 +621,14 @@
         <v>12</v>
       </c>
       <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -633,11 +651,14 @@
         <v>5</v>
       </c>
       <c r="H7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -660,11 +681,14 @@
         <v>3</v>
       </c>
       <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -687,11 +711,14 @@
         <v>5</v>
       </c>
       <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -714,11 +741,14 @@
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2">
+        <f>SUM(B10:H10)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -741,11 +771,14 @@
         <v>3</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <f>SUM(B11:H11)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -768,11 +801,14 @@
         <v>4</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2">
+        <f>SUM(B12:H12)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -795,11 +831,14 @@
         <v>0</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f>SUM(B13:H13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -820,7 +859,7 @@
         <v>49</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" ref="F14:H14" si="1">SUM(F2:F13)</f>
+        <f t="shared" ref="F14:I14" si="1">SUM(F2:F13)</f>
         <v>37</v>
       </c>
       <c r="G14" s="2">
@@ -829,7 +868,11 @@
       </c>
       <c r="H14" s="2">
         <f>SUM(H2:H13)</f>
-        <v>269</v>
+        <v>46</v>
+      </c>
+      <c r="I14" s="2">
+        <f>SUM(I2:I13)</f>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data for SNMV and OPM
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/svmvHomiEdad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Sistema_de_Notificacion_de_Muertes_Violentas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Sistema_de_Notificacion_de_Muertes_Violentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7471904-2355-45F9-8456-7E7BBCF1E4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C75CEB-0560-457D-B682-AFEB59363DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320" xr2:uid="{158DB65A-6E55-0941-A295-AA375E07226E}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{158DB65A-6E55-0941-A295-AA375E07226E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +99,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,9 +146,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +186,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +292,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +434,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA841438-AD1F-5942-BFE3-B2D151D6E29E}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,11 +475,14 @@
       <c r="H1" s="2">
         <v>2023</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="I1" s="2">
+        <v>2024</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -498,17 +502,20 @@
         <v>3</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="2">
         <v>3</v>
       </c>
       <c r="I2" s="2">
-        <f>SUM(B2:H2)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2">
+        <f>SUM(B2:I2)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -534,11 +541,14 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <f>SUM(B3:I3)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -558,17 +568,20 @@
         <v>7</v>
       </c>
       <c r="G4" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <v>2</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J14" si="0">SUM(B4:I4)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -594,11 +607,14 @@
         <v>6</v>
       </c>
       <c r="I5" s="2">
+        <v>9</v>
+      </c>
+      <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -624,11 +640,14 @@
         <v>3</v>
       </c>
       <c r="I6" s="2">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -654,11 +673,14 @@
         <v>6</v>
       </c>
       <c r="I7" s="2">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -684,11 +706,14 @@
         <v>5</v>
       </c>
       <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -714,11 +739,14 @@
         <v>5</v>
       </c>
       <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -744,11 +772,14 @@
         <v>3</v>
       </c>
       <c r="I10" s="2">
-        <f>SUM(B10:H10)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -774,11 +805,14 @@
         <v>1</v>
       </c>
       <c r="I11" s="2">
-        <f>SUM(B11:H11)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -804,11 +838,14 @@
         <v>11</v>
       </c>
       <c r="I12" s="2">
-        <f>SUM(B12:H12)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>8</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -834,11 +871,14 @@
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <f>SUM(B13:H13)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -859,20 +899,23 @@
         <v>49</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" ref="F14:I14" si="1">SUM(F2:F13)</f>
+        <f t="shared" ref="F14" si="1">SUM(F2:F13)</f>
         <v>37</v>
       </c>
       <c r="G14" s="2">
         <f>SUM(G2:G13)</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H14" s="2">
         <f>SUM(H2:H13)</f>
         <v>46</v>
       </c>
       <c r="I14" s="2">
-        <f>SUM(I2:I13)</f>
-        <v>315</v>
+        <v>60</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>